<commit_message>
joint_routes: fixed xlsx template.
</commit_message>
<xml_diff>
--- a/htdocs/assets/joint_routes.xlsx
+++ b/htdocs/assets/joint_routes.xlsx
@@ -5,10 +5,11 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="joint_routes" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="scores" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="50">
   <si>
     <t xml:space="preserve">№</t>
   </si>
@@ -43,58 +44,133 @@
     <t xml:space="preserve">Длит.</t>
   </si>
   <si>
-    <t xml:space="preserve">Посещ.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Факт</t>
+    <t xml:space="preserve">Длит. без учета перем.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Кол-во посещ.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Оценка в баллах</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Оценка в %</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Сильные стороны</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Области для развития</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Рекомендации для развития</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Автор</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Код клиента</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Название клиента</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Адрес клиента</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Канал рынка</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Категория клиента</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Регион</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Город</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Торговая сеть</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Тип торговой сети</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Критерий оценки</t>
   </si>
   <si>
     <t xml:space="preserve">Оценка</t>
   </si>
   <si>
-    <t xml:space="preserve">SLA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Сильные стороны</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Области для развития</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Рекомендации для развития</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Автор</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">11</t>
-  </si>
-  <si>
-    <t xml:space="preserve">12</t>
-  </si>
-  <si>
-    <t xml:space="preserve">14</t>
-  </si>
-  <si>
-    <t xml:space="preserve">15</t>
+    <t xml:space="preserve">Комментарий к оценке</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Вес оценки</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Комментарий к посещению</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Итоговая оценка в баллах</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Итоговая оценка в %</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">24</t>
   </si>
 </sst>
 </file>
@@ -336,12 +412,12 @@
   </sheetPr>
   <dimension ref="A1:O1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B3" activeCellId="0" sqref="B3"/>
+      <selection pane="bottomRight" activeCell="K2" activeCellId="0" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.4921875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -463,4 +539,203 @@
     <oddFooter/>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:X2"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="B2" activeCellId="0" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.4921875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="4.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="12.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="17.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="3" width="18.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="4" width="11.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="3" width="22.05"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="3" width="46.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="8" style="3" width="12.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="3" width="11.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="3" width="16.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="3" width="12.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="3" width="31.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="4" width="9.19"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="3" width="31.25"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="17" min="17" style="4" width="8.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="3" width="31.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="19" style="4" width="9.19"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="21" style="3" width="39.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="3" width="19.65"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="66" min="25" style="5" width="8.5"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1017" min="67" style="6" width="8.5"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="36.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="I1" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="J1" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="K1" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="L1" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="M1" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="N1" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="O1" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="P1" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q1" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="R1" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="S1" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="T1" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="U1" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="V1" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="W1" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="X1" s="9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="10" t="n">
+        <v>2</v>
+      </c>
+      <c r="C2" s="10" t="n">
+        <v>3</v>
+      </c>
+      <c r="D2" s="11" t="n">
+        <v>4</v>
+      </c>
+      <c r="E2" s="11" t="n">
+        <v>5</v>
+      </c>
+      <c r="F2" s="11" t="n">
+        <v>6</v>
+      </c>
+      <c r="G2" s="11" t="n">
+        <v>7</v>
+      </c>
+      <c r="H2" s="11" t="n">
+        <v>8</v>
+      </c>
+      <c r="I2" s="11" t="n">
+        <v>9</v>
+      </c>
+      <c r="J2" s="11" t="n">
+        <v>10</v>
+      </c>
+      <c r="K2" s="11" t="n">
+        <v>11</v>
+      </c>
+      <c r="L2" s="11" t="n">
+        <v>12</v>
+      </c>
+      <c r="M2" s="11" t="n">
+        <v>13</v>
+      </c>
+      <c r="N2" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="O2" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="P2" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q2" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="R2" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="S2" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="T2" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="U2" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="V2" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="W2" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="X2" s="11" t="s">
+        <v>49</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Обычный"&amp;Kffffff&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Обычный"&amp;KffffffСтраница &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>